<commit_message>
Upd 12_5_23: font and format changes
</commit_message>
<xml_diff>
--- a/excel_project.xlsx
+++ b/excel_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guttman\Desktop\mis_excel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A770DA-EB1A-46A1-B249-1E0E3174DB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14150981-13F2-4C9D-984B-0B3B69B9ADCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Collection" sheetId="1" r:id="rId1"/>
@@ -9839,7 +9839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EC2443-40CB-446D-BB83-686BA2887BDC}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="69" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -9850,13 +9850,13 @@
     <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -10670,7 +10670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1D3D86-40A7-4240-9003-D7BBC33CF772}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="65" workbookViewId="0">
+    <sheetView zoomScale="65" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Upd 12_5_23: Reformatting charts
</commit_message>
<xml_diff>
--- a/excel_project.xlsx
+++ b/excel_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guttman\Desktop\mis_excel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A63B5E0-8355-4BAB-8AB7-AC80F94E09F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A770DA-EB1A-46A1-B249-1E0E3174DB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Collection" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>Financial Strength</t>
   </si>
   <si>
-    <t>This test allows you to differentiate between companies that are on the ropes or financially strong.</t>
-  </si>
-  <si>
     <t>E. Total Liabilities vs Total Assets</t>
   </si>
   <si>
@@ -140,6 +137,10 @@
   <si>
     <t>A. Net income should be positive.</t>
   </si>
+  <si>
+    <t>This test allows you to differentiate between companies that are on the ropes or 
+financially strong.</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,68 +161,6 @@
       <sz val="8"/>
       <name val="Calisto MT"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calisto MT"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calisto MT"/>
-      <family val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -253,8 +192,67 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
-      <color theme="6" tint="0.79998168889431442"/>
+      <color theme="1"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Bahnschrift SemiBold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Franklin Gothic Demi Cond"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Demi Cond"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Franklin Gothic Demi Cond"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Segoe UI Semibold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Segoe UI Semibold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Segoe UI Semibold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Bahnschrift SemiLight"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Bahnschrift"/>
       <family val="2"/>
     </font>
@@ -262,15 +260,29 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calisto MT"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="6" tint="0.79998168889431442"/>
       <name val="Bahnschrift"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Segoe UI Light"/>
-      <family val="2"/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calisto MT"/>
+      <family val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -329,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -695,11 +707,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -710,138 +750,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,11 +885,17 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -862,52 +903,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -931,19 +927,46 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -952,10 +975,61 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5243,7 +5317,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-7417-45DB-BBFF-726AC7094D94}"/>
                   </c:ext>
@@ -9174,578 +9248,578 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="61" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A27" zoomScale="61" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="40">
         <v>45138</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="41">
         <v>45046</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="42">
         <v>44957</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="41">
         <v>44865</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="44">
         <v>39782000</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="45">
         <v>37017000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="45">
         <v>38625000</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="45">
         <v>37200000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="46">
         <v>255121000</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="47">
         <v>245053000</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="47">
         <v>243457000</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="47">
         <v>247656000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="46">
         <v>169562000</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="47">
         <v>165588000</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="47">
         <v>159466000</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="47">
         <v>167273000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A6" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="46">
         <v>85559000</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="47">
         <v>79465000</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="47">
         <v>83991000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="47">
         <v>80383000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="46">
         <v>14041000</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="47">
         <v>7891000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="47">
         <v>1673000</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="47">
         <v>6275000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="46">
         <v>13568000</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="47">
         <v>4633000</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="47">
         <v>13403000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="47">
         <v>6458000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="49">
         <v>3270000</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="50">
         <v>1713000</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="50">
         <v>-2812000</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="50">
         <v>-2104000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="40">
         <v>44957</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="51">
         <v>44592</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="51">
         <v>44227</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="51">
         <v>43861</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A11" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="44">
         <v>147568000</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="45">
         <v>143754000</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="45">
         <v>138836000</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="45">
         <v>129359000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A12" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="46">
         <v>243457000</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="47">
         <v>244860000</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="47">
         <v>252496000</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="47">
         <v>236495000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A13" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="46">
         <v>159466000</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="47">
         <v>152969000</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="47">
         <v>164965000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="47">
         <v>154943000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A14" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="46">
         <v>76693000</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="47">
         <v>83253000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="47">
         <v>81298000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="47">
         <v>74669000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A15" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="53">
         <v>11680000</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="47">
         <v>13673000</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="47">
         <v>13510000</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="47">
         <v>14881000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A16" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="46">
         <v>29101000</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="47">
         <v>24181000</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="47">
         <v>36074000</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="47">
         <v>25255000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A17" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="46">
         <v>-5660000</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="47">
         <v>-4662000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="47">
         <v>9886000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="47">
         <v>1828000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37" t="s">
+    <row r="18" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A18" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
     </row>
-    <row r="19" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A19" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="54">
         <v>45169</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="41">
         <v>45077</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="42">
         <v>44985</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="41">
         <v>44957</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A20" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="44">
         <v>9720000</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="45">
         <v>6473000</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="45">
         <v>6843000</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="45">
         <v>6843000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A21" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="46">
         <v>68994000</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="47">
         <v>66752000</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="47">
         <v>66848000</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="47">
         <v>66848000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A22" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="46">
         <v>43936000</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="47">
         <v>43179000</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="47">
         <v>44049000</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="47">
         <v>44049000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A23" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="46">
         <v>25058000</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="47">
         <v>23568000</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="47">
         <v>22794000</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="47">
         <v>22794000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A24" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="46">
         <v>6292000</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="47">
         <v>2160000</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="47">
         <v>1302000</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="47">
         <v>1466000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A25" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="46">
         <v>3725000</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="47">
         <v>1541000</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="47">
         <v>3192000</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="47">
         <v>2610000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
+    <row r="26" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A26" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="49">
         <v>1236000</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="50">
         <v>-476000</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="50">
         <v>2032000</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="50">
         <v>690000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A27" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="54">
         <v>45169</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="51">
         <v>44804</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="51">
         <v>44439</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="51">
         <v>44074</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="44">
         <v>29704000</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="45">
         <v>27572000</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="45">
         <v>25245000</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="45">
         <v>21822000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A29" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="46">
         <v>68994000</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="47">
         <v>64166000</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="47">
         <v>59268000</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="47">
         <v>55556000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="46">
         <v>43936000</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="47">
         <v>43519000</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="47">
         <v>41190000</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="47">
         <v>36851000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A31" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="46">
         <v>25058000</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="47">
         <v>20642000</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="47">
         <v>17564000</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="47">
         <v>18284000</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A32" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="53">
         <v>6292000</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="47">
         <v>5844000</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="47">
         <v>5007000</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="47">
         <v>4002000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A33" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="46">
         <v>11068000</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="47">
         <v>7392000</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="47">
         <v>8958000</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="47">
         <v>8861000</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A34" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="46">
         <v>3482000</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="47">
         <v>-806000</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="47">
         <v>-1065000</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="47">
         <v>3823000</v>
       </c>
     </row>
@@ -9765,806 +9839,808 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EC2443-40CB-446D-BB83-686BA2887BDC}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="D1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:14" ht="23.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="16" t="s">
-        <v>23</v>
+      <c r="K1" s="33"/>
+      <c r="L1" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="33"/>
+      <c r="N1" s="32" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="18">
         <f>'Data Collection'!$B$10</f>
         <v>44957</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="19">
         <f>'Data Collection'!$B$11</f>
         <v>147568000</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="19">
         <f>'Data Collection'!$B$12</f>
         <v>243457000</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="19">
         <f>'Data Collection'!$D$13</f>
         <v>164965000</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="19">
         <f>'Data Collection'!$B$13</f>
         <v>159466000</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="19">
         <f>'Data Collection'!$B$15</f>
         <v>11680000</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="19">
         <f>'Data Collection'!$B$16</f>
         <v>29101000</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="19">
         <f>'Data Collection'!$B$17</f>
         <v>-5660000</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="5">
+      <c r="K2" s="17"/>
+      <c r="L2" s="19">
         <f>'Data Collection'!$B$13</f>
         <v>159466000</v>
       </c>
-      <c r="M2" s="38"/>
-      <c r="N2" s="31">
+      <c r="M2" s="17"/>
+      <c r="N2" s="20">
         <f>Process!H2/Process!E2</f>
         <v>4.7975617870917656E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="24">
+    <row r="3" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="18">
         <f>'Data Collection'!$C$10</f>
         <v>44592</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="19">
         <f>'Data Collection'!$C$11</f>
         <v>143754000</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="19">
         <f>'Data Collection'!$C$12</f>
         <v>244860000</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="19">
         <f>'Data Collection'!$C$13</f>
         <v>152969000</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="19">
         <f>'Data Collection'!$C$14</f>
         <v>83253000</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="19">
         <f>'Data Collection'!$C$15</f>
         <v>13673000</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="19">
         <f>'Data Collection'!$C$16</f>
         <v>24181000</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="19">
         <f>'Data Collection'!$C$17</f>
         <v>-4662000</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="5">
+      <c r="K3" s="17"/>
+      <c r="L3" s="19">
         <f>'Data Collection'!$C$14</f>
         <v>83253000</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="31">
+      <c r="M3" s="17"/>
+      <c r="N3" s="20">
         <f>Process!H3/Process!E3</f>
         <v>5.5840071877807727E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="24">
+    <row r="4" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="18">
         <f>'Data Collection'!$D$10</f>
         <v>44227</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="19">
         <f>'Data Collection'!$D$11</f>
         <v>138836000</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="19">
         <f>'Data Collection'!$C$12</f>
         <v>244860000</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="19">
         <f>'Data Collection'!$D$13</f>
         <v>164965000</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="19">
         <f>'Data Collection'!$D$14</f>
         <v>81298000</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="19">
         <f>'Data Collection'!$D$15</f>
         <v>13510000</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="19">
         <f>'Data Collection'!$D$16</f>
         <v>36074000</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="19">
         <f>'Data Collection'!$D$17</f>
         <v>9886000</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="5">
+      <c r="K4" s="17"/>
+      <c r="L4" s="19">
         <f>'Data Collection'!$D$14</f>
         <v>81298000</v>
       </c>
-      <c r="M4" s="38"/>
-      <c r="N4" s="31">
+      <c r="M4" s="17"/>
+      <c r="N4" s="20">
         <f>Process!H4 / Process!E4</f>
         <v>5.5174385363064606E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="24">
+    <row r="5" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="18">
         <f>'Data Collection'!$E$10</f>
         <v>43861</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="19">
         <f>'Data Collection'!$E$11</f>
         <v>129359000</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="19">
         <f>'Data Collection'!$E$12</f>
         <v>236495000</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="19">
         <f>'Data Collection'!$E$13</f>
         <v>154943000</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="19">
         <f>'Data Collection'!$E$14</f>
         <v>74669000</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="19">
         <f>'Data Collection'!$E$15</f>
         <v>14881000</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="19">
         <f>'Data Collection'!$E$16</f>
         <v>25255000</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="19">
         <f>'Data Collection'!$E$17</f>
         <v>1828000</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="5">
+      <c r="K5" s="17"/>
+      <c r="L5" s="19">
         <f>'Data Collection'!$E$14</f>
         <v>74669000</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="31">
+      <c r="M5" s="17"/>
+      <c r="N5" s="20">
         <f>Process!H5 / Process!E5</f>
         <v>6.2923106196748346E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="18">
         <f>'Data Collection'!$B$2</f>
         <v>45138</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="19">
         <f>'Data Collection'!$B$3</f>
         <v>39782000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="19">
         <f>'Data Collection'!$B$4</f>
         <v>255121000</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="19">
         <f>'Data Collection'!$B$5</f>
         <v>169562000</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="19">
         <f>'Data Collection'!$B$6</f>
         <v>85559000</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="19">
         <f>'Data Collection'!$B$7</f>
         <v>14041000</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="19">
         <f>'Data Collection'!$B$8</f>
         <v>13568000</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="19">
         <f>'Data Collection'!$B$9</f>
         <v>3270000</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="5">
+      <c r="K6" s="17"/>
+      <c r="L6" s="19">
         <f>'Data Collection'!$B$6</f>
         <v>85559000</v>
       </c>
-      <c r="M6" s="38"/>
-      <c r="N6" s="31">
+      <c r="M6" s="17"/>
+      <c r="N6" s="20">
         <f>Process!H6 / Process!E6</f>
         <v>5.5036629677682351E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="24">
+    <row r="7" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18">
         <f>'Data Collection'!$C$2</f>
         <v>45046</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="19">
         <f>'Data Collection'!$C$3</f>
         <v>37017000</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="19">
         <f>'Data Collection'!$C$4</f>
         <v>245053000</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="19">
         <f>'Data Collection'!$C$5</f>
         <v>165588000</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="19">
         <f>'Data Collection'!$C$6</f>
         <v>79465000</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="19">
         <f>'Data Collection'!$C$7</f>
         <v>7891000</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="19">
         <f>'Data Collection'!$C$8</f>
         <v>4633000</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="19">
         <f>'Data Collection'!$C$9</f>
         <v>1713000</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="5">
+      <c r="K7" s="17"/>
+      <c r="L7" s="19">
         <f>'Data Collection'!$C$6</f>
         <v>79465000</v>
       </c>
-      <c r="M7" s="38"/>
-      <c r="N7" s="31">
+      <c r="M7" s="17"/>
+      <c r="N7" s="20">
         <f>Process!H7 / Process!E7</f>
         <v>3.2201197292014379E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="24">
+    <row r="8" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="18">
         <f>'Data Collection'!$D$2</f>
         <v>44957</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="19">
         <f>'Data Collection'!$D$3</f>
         <v>38625000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="19">
         <f>'Data Collection'!$D$4</f>
         <v>243457000</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="19">
         <f>'Data Collection'!$D$5</f>
         <v>159466000</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="19">
         <f>'Data Collection'!$D$6</f>
         <v>83991000</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="19">
         <f>'Data Collection'!$D$7</f>
         <v>1673000</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="19">
         <f>'Data Collection'!$D$8</f>
         <v>13403000</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="19">
         <f>'Data Collection'!$D$9</f>
         <v>-2812000</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="5">
+      <c r="K8" s="17"/>
+      <c r="L8" s="19">
         <f>'Data Collection'!$D$6</f>
         <v>83991000</v>
       </c>
-      <c r="M8" s="38"/>
-      <c r="N8" s="31">
+      <c r="M8" s="17"/>
+      <c r="N8" s="20">
         <f>H8 / E8</f>
         <v>6.8718500597641473E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="28">
+    <row r="9" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="21">
         <f>'Data Collection'!$E$2</f>
         <v>44865</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="22">
         <f>'Data Collection'!$E$3</f>
         <v>37200000</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="22">
         <f>'Data Collection'!$E$4</f>
         <v>247656000</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="22">
         <f>'Data Collection'!$E$5</f>
         <v>167273000</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="22">
         <f>'Data Collection'!$E$6</f>
         <v>80383000</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="22">
         <f>'Data Collection'!$E$7</f>
         <v>6275000</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="22">
         <f>'Data Collection'!$E$8</f>
         <v>6458000</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="22">
         <f>'Data Collection'!$E$9</f>
         <v>-2104000</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="18">
+      <c r="K9" s="17"/>
+      <c r="L9" s="22">
         <f>'Data Collection'!$E$6</f>
         <v>80383000</v>
       </c>
-      <c r="M9" s="38"/>
-      <c r="N9" s="32">
+      <c r="M9" s="17"/>
+      <c r="N9" s="23">
         <f>Process!H9 / Process!E9</f>
         <v>2.5337565009529345E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="24">
         <f>'Data Collection'!$B$27</f>
         <v>45169</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="25">
         <f>'Data Collection'!$B$28</f>
         <v>29704000</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="25">
         <f>'Data Collection'!$B$29</f>
         <v>68994000</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="25">
         <f>'Data Collection'!$B$30</f>
         <v>43936000</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="25">
         <f>'Data Collection'!$B$31</f>
         <v>25058000</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="25">
         <f>'Data Collection'!$B$32</f>
         <v>6292000</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="25">
         <f>'Data Collection'!$B$33</f>
         <v>11068000</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="25">
         <f>'Data Collection'!$B$34</f>
         <v>3482000</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="30">
+      <c r="K10" s="17"/>
+      <c r="L10" s="25">
         <f>'Data Collection'!$B$31</f>
         <v>25058000</v>
       </c>
-      <c r="M10" s="38"/>
-      <c r="N10" s="31">
+      <c r="M10" s="17"/>
+      <c r="N10" s="26">
         <f>Process!H10/Process!E10</f>
         <v>9.1196335913267826E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="24">
+    <row r="11" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="18">
         <f>'Data Collection'!$C$27</f>
         <v>44804</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="19">
         <f>'Data Collection'!$C$28</f>
         <v>27572000</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="19">
         <f>'Data Collection'!$C$29</f>
         <v>64166000</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="19">
         <f>'Data Collection'!$C$30</f>
         <v>43519000</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="19">
         <f>'Data Collection'!$C$31</f>
         <v>20642000</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="19">
         <f>'Data Collection'!$C$32</f>
         <v>5844000</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="19">
         <f>'Data Collection'!$C$33</f>
         <v>7392000</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="19">
         <f>'Data Collection'!$C$34</f>
         <v>-806000</v>
       </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="5">
+      <c r="K11" s="17"/>
+      <c r="L11" s="19">
         <f>'Data Collection'!$C$31</f>
         <v>20642000</v>
       </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="31">
+      <c r="M11" s="17"/>
+      <c r="N11" s="20">
         <f>Process!H11/Process!E11</f>
         <v>9.1076270922295297E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="24">
+    <row r="12" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="18">
         <f>'Data Collection'!$D$27</f>
         <v>44439</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="19">
         <f>'Data Collection'!$D$28</f>
         <v>25245000</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="19">
         <f>'Data Collection'!$D$29</f>
         <v>59268000</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="19">
         <f>'Data Collection'!$D$30</f>
         <v>41190000</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="19">
         <f>'Data Collection'!$D$31</f>
         <v>17564000</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="19">
         <f>'Data Collection'!$D$32</f>
         <v>5007000</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="19">
         <f>'Data Collection'!$D$33</f>
         <v>8958000</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="19">
         <f>'Data Collection'!$D$34</f>
         <v>-1065000</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="5">
+      <c r="K12" s="17"/>
+      <c r="L12" s="19">
         <f>'Data Collection'!$D$31</f>
         <v>17564000</v>
       </c>
-      <c r="M12" s="38"/>
-      <c r="N12" s="31">
+      <c r="M12" s="17"/>
+      <c r="N12" s="20">
         <f>Process!H12 / Process!E12</f>
         <v>8.4480664102044953E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="24">
+    <row r="13" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="18">
         <f>'Data Collection'!$E$27</f>
         <v>44074</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="19">
         <f>'Data Collection'!$E$28</f>
         <v>21822000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="19">
         <f>'Data Collection'!$E$29</f>
         <v>55556000</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="19">
         <f>'Data Collection'!$E$30</f>
         <v>36851000</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="19">
         <f>'Data Collection'!$E$31</f>
         <v>18284000</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="19">
         <f>'Data Collection'!$E$32</f>
         <v>4002000</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="19">
         <f>'Data Collection'!$E$33</f>
         <v>8861000</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="19">
         <f>'Data Collection'!$E$34</f>
         <v>3823000</v>
       </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="5">
+      <c r="K13" s="17"/>
+      <c r="L13" s="19">
         <f>'Data Collection'!$E$31</f>
         <v>18284000</v>
       </c>
-      <c r="M13" s="38"/>
-      <c r="N13" s="31">
+      <c r="M13" s="17"/>
+      <c r="N13" s="20">
         <f>Process!H13 / Process!E13</f>
         <v>7.2035423716610272E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
-      <c r="B14" s="39" t="s">
+    <row r="14" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="34"/>
+      <c r="B14" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="18">
         <f>'Data Collection'!$B$19</f>
         <v>45169</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="19">
         <f>'Data Collection'!$B$20</f>
         <v>9720000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="19">
         <f>'Data Collection'!$B$21</f>
         <v>68994000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="19">
         <f>'Data Collection'!$B$22</f>
         <v>43936000</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="19">
         <f>'Data Collection'!$B$23</f>
         <v>25058000</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="19">
         <f>'Data Collection'!$B$24</f>
         <v>6292000</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="19">
         <f>'Data Collection'!$B$25</f>
         <v>3725000</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="19">
         <f>'Data Collection'!$B$26</f>
         <v>1236000</v>
       </c>
-      <c r="K14" s="38"/>
-      <c r="L14" s="5">
+      <c r="K14" s="17"/>
+      <c r="L14" s="19">
         <f>'Data Collection'!$B$23</f>
         <v>25058000</v>
       </c>
-      <c r="M14" s="38"/>
-      <c r="N14" s="31">
+      <c r="M14" s="17"/>
+      <c r="N14" s="20">
         <f>Process!H14 / Process!E14</f>
         <v>9.1196335913267826E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="24">
+    <row r="15" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="18">
         <f>'Data Collection'!$C$19</f>
         <v>45077</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="19">
         <f>'Data Collection'!$C$20</f>
         <v>6473000</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="19">
         <f>'Data Collection'!$C$21</f>
         <v>66752000</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="19">
         <f>'Data Collection'!$C$22</f>
         <v>43179000</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="19">
         <f>'Data Collection'!$C$23</f>
         <v>23568000</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="19">
         <f>'Data Collection'!$C$24</f>
         <v>2160000</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="19">
         <f>'Data Collection'!$C$25</f>
         <v>1541000</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="19">
         <f>'Data Collection'!$C$26</f>
         <v>-476000</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="5">
+      <c r="K15" s="17"/>
+      <c r="L15" s="19">
         <f>'Data Collection'!$C$23</f>
         <v>23568000</v>
       </c>
-      <c r="M15" s="38"/>
-      <c r="N15" s="31">
+      <c r="M15" s="17"/>
+      <c r="N15" s="20">
         <f>Process!H15 / Process!E15</f>
         <v>3.235858101629914E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="24">
+    <row r="16" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="18">
         <f>'Data Collection'!$D$19</f>
         <v>44985</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="19">
         <f>'Data Collection'!$D$20</f>
         <v>6843000</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="19">
         <f>'Data Collection'!$D$21</f>
         <v>66848000</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="19">
         <f>'Data Collection'!$D$22</f>
         <v>44049000</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="19">
         <f>'Data Collection'!$D$23</f>
         <v>22794000</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="19">
         <f>'Data Collection'!$D$24</f>
         <v>1302000</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="19">
         <f>'Data Collection'!$D$25</f>
         <v>3192000</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="19">
         <f>'Data Collection'!$D$26</f>
         <v>2032000</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="5">
+      <c r="K16" s="17"/>
+      <c r="L16" s="19">
         <f>'Data Collection'!$D$23</f>
         <v>22794000</v>
       </c>
-      <c r="M16" s="38"/>
-      <c r="N16" s="31">
+      <c r="M16" s="17"/>
+      <c r="N16" s="27">
         <f>H16 / E16</f>
         <v>1.9477022498803256E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="24">
+    <row r="17" spans="1:14" ht="27.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="18">
         <f>'Data Collection'!$E$19</f>
         <v>44957</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="19">
         <f>'Data Collection'!$E$20</f>
         <v>6843000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="19">
         <f>'Data Collection'!$E$21</f>
         <v>66848000</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="19">
         <f>'Data Collection'!$E$22</f>
         <v>44049000</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="19">
         <f>'Data Collection'!$E$23</f>
         <v>22794000</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="19">
         <f>'Data Collection'!$E$24</f>
         <v>1466000</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="19">
         <f>'Data Collection'!$E$25</f>
         <v>2610000</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="19">
         <f>'Data Collection'!$E$26</f>
         <v>690000</v>
       </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="5">
+      <c r="K17" s="17"/>
+      <c r="L17" s="19">
         <f>'Data Collection'!$E$23</f>
         <v>22794000</v>
       </c>
-      <c r="M17" s="38"/>
-      <c r="N17" s="32">
+      <c r="M17" s="17"/>
+      <c r="N17" s="28">
         <f>Process!H17 / Process!E17</f>
         <v>2.1930349449497368E-2</v>
       </c>
@@ -10594,583 +10670,602 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1D3D86-40A7-4240-9003-D7BBC33CF772}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="65" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="65" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6328125" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" customWidth="1"/>
     <col min="3" max="4" width="15.6328125" customWidth="1"/>
     <col min="5" max="5" width="32.90625" customWidth="1"/>
     <col min="6" max="7" width="15.6328125" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="8" max="8" width="40.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:8" ht="14" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="94" t="s">
+    <row r="1" spans="1:8" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" ht="14" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="105"/>
     </row>
-    <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
+    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="107"/>
     </row>
-    <row r="4" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="109"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="64" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="15" t="str">
         <f>Process!A2 &amp;CHAR(10)&amp;COUNTIF(C11:C42, "Pass*") &amp; " out of " &amp; COUNTIF(C11:C42, "Pass*")+COUNTIF(C11:C42, "Fail*")</f>
         <v>Walmart
 7 out of 8</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64" t="str">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="str">
         <f>Process!A10 &amp;CHAR(10)&amp;COUNTIF(F12:F42, "Pass*") &amp; " out of " &amp; COUNTIF(F12:F42, "Pass*")+COUNTIF(F12:F42, "Fail*")</f>
         <v>Costco
 7 out of 8</v>
       </c>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="66" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
+    <row r="12" spans="1:8" ht="23.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="89" t="str">
+      <c r="A13" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="55" t="str">
         <f>IF(Process!H9 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D13" s="95" t="str">
+      <c r="D13" s="56" t="str">
         <f>DOLLAR(Process!H9,0)</f>
         <v>$6,275,000</v>
       </c>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89" t="str">
+      <c r="E13" s="55"/>
+      <c r="F13" s="55" t="str">
         <f>IF(Process!H17 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G13" s="95" t="str">
+      <c r="G13" s="56" t="str">
         <f>DOLLAR(Process!H17,0)</f>
         <v>$1,466,000</v>
       </c>
-      <c r="H13" s="89"/>
+      <c r="H13" s="55"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
+    <row r="14" spans="1:8" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
     </row>
     <row r="15" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="89" t="str">
+      <c r="A15" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="67"/>
+      <c r="C15" s="55" t="str">
         <f>IF(Process!I9 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D15" s="95" t="str">
+      <c r="D15" s="56" t="str">
         <f>DOLLAR(Process!I9,0)</f>
         <v>$6,458,000</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89" t="str">
+      <c r="E15" s="55"/>
+      <c r="F15" s="55" t="str">
         <f>IF(Process!I17 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G15" s="95" t="str">
+      <c r="G15" s="56" t="str">
         <f>DOLLAR(Process!I17,0)</f>
         <v>$2,610,000</v>
       </c>
-      <c r="H15" s="89"/>
+      <c r="H15" s="55"/>
     </row>
     <row r="16" spans="1:8" ht="22" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="89" t="str">
+      <c r="A17" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="55" t="str">
         <f>IF(Process!N9 &gt; 1%, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D17" s="90">
+      <c r="D17" s="57">
         <f>Process!N9</f>
         <v>2.5337565009529345E-2</v>
       </c>
-      <c r="E17" s="90"/>
-      <c r="F17" s="89" t="str">
+      <c r="E17" s="57"/>
+      <c r="F17" s="55" t="str">
         <f>IF(Process!N17 &gt; 1%, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G17" s="90">
+      <c r="G17" s="57">
         <f>Process!N17</f>
         <v>2.1930349449497368E-2</v>
       </c>
-      <c r="H17" s="89"/>
+      <c r="H17" s="55"/>
     </row>
     <row r="18" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
     </row>
     <row r="19" spans="1:8" ht="18.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="81" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="82"/>
-      <c r="C19" s="41" t="str">
+      <c r="A19" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="70"/>
+      <c r="C19" s="58" t="str">
         <f>IF(Process!I9 &gt; Process!H9, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D19" s="58" t="str">
+      <c r="D19" s="59" t="str">
         <f>"Cash Flow= " &amp; DOLLAR(Process!I9,0) &amp;CHAR(10)&amp; " Net Income= " &amp; DOLLAR(Process!H9,0)</f>
         <v>Cash Flow= $6,458,000
  Net Income= $6,275,000</v>
       </c>
-      <c r="E19" s="59"/>
-      <c r="F19" s="41" t="str">
+      <c r="E19" s="60"/>
+      <c r="F19" s="58" t="str">
         <f>IF(Process!I17 &gt; Process!H17, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G19" s="58" t="str">
+      <c r="G19" s="59" t="str">
         <f>"Cash Flow= " &amp; DOLLAR(Process!I17,0) &amp;CHAR(10)&amp; " Net Income= " &amp; DOLLAR(Process!H17,0)</f>
         <v>Cash Flow= $2,610,000
  Net Income= $1,466,000</v>
       </c>
-      <c r="H19" s="59"/>
+      <c r="H19" s="60"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="83"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="61"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="63"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="85"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="63"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="66"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="68" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="70"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="73"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="12.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="50"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="94"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="53"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="97"/>
     </row>
-    <row r="26" spans="1:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="56"/>
+    <row r="26" spans="1:8" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="99"/>
+      <c r="G26" s="99"/>
+      <c r="H26" s="100"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="41" t="str">
+      <c r="A27" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="67"/>
+      <c r="C27" s="58" t="str">
         <f>IF(Process!E9 &gt; Process!F9, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D27" s="58" t="str">
+      <c r="D27" s="59" t="str">
         <f>"Assets = " &amp; DOLLAR(Process!E9,0) &amp; CHAR(10)&amp; " Liabilities = "&amp;DOLLAR(Process!F9,0)</f>
         <v>Assets = $247,656,000
  Liabilities = $167,273,000</v>
       </c>
-      <c r="E27" s="59"/>
-      <c r="F27" s="41" t="str">
+      <c r="E27" s="60"/>
+      <c r="F27" s="58" t="str">
         <f>IF(Process!E17 &gt; Process!F17, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G27" s="58" t="str">
+      <c r="G27" s="59" t="str">
         <f>"Assets = " &amp; DOLLAR(Process!E17,0) &amp; CHAR(10)&amp; " Liabilities = "&amp;DOLLAR(Process!F17,0)</f>
         <v>Assets = $66,848,000
  Liabilities = $44,049,000</v>
       </c>
-      <c r="H27" s="59"/>
+      <c r="H27" s="60"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="61"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="63"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="63"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="66"/>
     </row>
     <row r="30" spans="1:8" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="41" t="str">
+      <c r="A30" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="67"/>
+      <c r="C30" s="58" t="str">
         <f>IF(Process!L9 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D30" s="43" t="str">
+      <c r="D30" s="82" t="str">
         <f>DOLLAR(Process!L9,0)</f>
         <v>$80,383,000</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="F30" s="41" t="str">
+      <c r="E30" s="83"/>
+      <c r="F30" s="58" t="str">
         <f>IF(Process!L17 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G30" s="43" t="str">
+      <c r="G30" s="82" t="str">
         <f>DOLLAR(Process!L17,0)</f>
         <v>$22,794,000</v>
       </c>
-      <c r="H30" s="44"/>
+      <c r="H30" s="83"/>
     </row>
     <row r="31" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="47"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="46"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="85"/>
     </row>
-    <row r="32" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="66" t="s">
+    <row r="32" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="75"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="66"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
+    <row r="33" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="75"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
+      <c r="A34" s="75"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="91"/>
+      <c r="H34" s="91"/>
     </row>
-    <row r="35" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="88"/>
+    <row r="35" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="75"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="91"/>
     </row>
-    <row r="36" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="88"/>
+    <row r="36" spans="1:8" ht="35.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="75"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="91"/>
+      <c r="H36" s="91"/>
     </row>
     <row r="37" spans="1:8" ht="24.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="34" t="str">
+      <c r="A37" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="77"/>
+      <c r="C37" s="5" t="str">
         <f>IF(Process!D9 &gt; 0, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D37" s="87" t="str">
+      <c r="D37" s="7" t="str">
         <f>DOLLAR(Process!D9,0)</f>
         <v>$37,200,000</v>
       </c>
-      <c r="E37" s="87"/>
-      <c r="F37" s="34" t="str">
+      <c r="E37" s="7"/>
+      <c r="F37" s="5" t="str">
         <f>IF(Process!D17 &gt; 0, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G37" s="87" t="str">
+      <c r="G37" s="7" t="str">
         <f>DOLLAR(Process!D17,0)</f>
         <v>$6,843,000</v>
       </c>
-      <c r="H37" s="87"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="68" t="s">
+      <c r="A38" s="75"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="70"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="73"/>
+    <row r="39" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="75"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="91" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
+    <row r="40" spans="1:8" ht="54.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="75"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="88"/>
+      <c r="E40" s="88"/>
+      <c r="F40" s="88"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="88"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="77"/>
-      <c r="C41" s="92" t="str">
+      <c r="A41" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="79"/>
+      <c r="C41" s="89" t="str">
         <f>IF(Process!I9 &gt; Process!F9, "Pass", "Fail")</f>
         <v>Fail</v>
       </c>
-      <c r="D41" s="93" t="str">
+      <c r="D41" s="90" t="str">
         <f>"Cash Flow = " &amp; DOLLAR(Process!I9, 0) &amp; CHAR(10)&amp; " Liabilities = " &amp; DOLLAR(Process!F9,0)</f>
         <v>Cash Flow = $6,458,000
  Liabilities = $167,273,000</v>
       </c>
-      <c r="E41" s="93"/>
-      <c r="F41" s="92" t="str">
+      <c r="E41" s="90"/>
+      <c r="F41" s="89" t="str">
         <f>IF(Process!I17 &gt; Process!F17, "Pass", "Fail")</f>
         <v>Fail</v>
       </c>
-      <c r="G41" s="93" t="str">
+      <c r="G41" s="90" t="str">
         <f>"Cash Flow = " &amp; DOLLAR(Process!I17, 0) &amp; CHAR(10)&amp; " Liabilities = " &amp; DOLLAR(Process!F17,0)</f>
         <v>Cash Flow = $2,610,000
  Liabilities = $44,049,000</v>
       </c>
-      <c r="H41" s="93"/>
+      <c r="H41" s="90"/>
     </row>
     <row r="42" spans="1:8" ht="30.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="78"/>
-      <c r="B42" s="79"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="93"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="93"/>
-      <c r="H42" s="93"/>
+      <c r="A42" s="80"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
     </row>
     <row r="43" spans="1:8" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C2:H4"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="D27:E29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G27:H29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:H31"/>
+    <mergeCell ref="C38:H39"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A41:B42"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B21"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:H42"/>
+    <mergeCell ref="D19:E21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:H21"/>
+    <mergeCell ref="C24:H26"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="G37:H37"/>
@@ -11185,36 +11280,17 @@
     <mergeCell ref="G15:H16"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C38:H39"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A41:B42"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B21"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:H42"/>
+    <mergeCell ref="A27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C2:H4"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="C5:E8"/>
     <mergeCell ref="F5:H8"/>
     <mergeCell ref="C9:H10"/>
     <mergeCell ref="C11:H12"/>
-    <mergeCell ref="D19:E21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:H21"/>
-    <mergeCell ref="C24:H26"/>
-    <mergeCell ref="A27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:E29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G27:H29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:H31"/>
-    <mergeCell ref="A30:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11224,8 +11300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2C5099-E488-45DC-8972-3201FC9593C4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="58" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+    <sheetView topLeftCell="A3" zoomScale="58" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Upd 12_5_23: data and chart updates
</commit_message>
<xml_diff>
--- a/excel_project.xlsx
+++ b/excel_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guttman\Desktop\mis_excel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14150981-13F2-4C9D-984B-0B3B69B9ADCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F842EA6F-6538-4487-95EC-06DF898B0455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Collection" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Walmart</t>
   </si>
@@ -141,6 +141,9 @@
     <t>This test allows you to differentiate between companies that are on the ropes or 
 financially strong.</t>
   </si>
+  <si>
+    <t>Return on Equity</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,13 +190,6 @@
     </font>
     <font>
       <sz val="20"/>
-      <color theme="1"/>
-      <name val="Bahnschrift"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Bahnschrift"/>
       <family val="2"/>
@@ -285,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,8 +336,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -735,11 +737,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -751,14 +768,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -787,249 +798,262 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1180,7 +1204,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Costco</c:v>
+            <c:strRef>
+              <c:f>Process!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Costco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
@@ -1289,7 +1321,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Walmart</c:v>
+            <c:strRef>
+              <c:f>Process!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Walmart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
@@ -1817,10 +1857,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="104"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="4"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1941,21 +1981,27 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Walmart</c:v>
+            <c:strRef>
+              <c:f>Process!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Walmart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
                   <a:schemeClr val="accent2">
-                    <a:shade val="58000"/>
                     <a:tint val="96000"/>
                     <a:lumMod val="104000"/>
                   </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
                   <a:schemeClr val="accent2">
-                    <a:shade val="58000"/>
                     <a:shade val="90000"/>
                     <a:lumMod val="90000"/>
                   </a:schemeClr>
@@ -1986,6 +2032,61 @@
             </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Process!$C$2:$C$5</c:f>
@@ -2038,21 +2139,27 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Costco</c:v>
+            <c:strRef>
+              <c:f>'Data Collection'!$A$18:$E$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Costco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:tint val="86000"/>
+                  <a:schemeClr val="accent6">
                     <a:tint val="96000"/>
                     <a:lumMod val="104000"/>
                   </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:tint val="86000"/>
+                  <a:schemeClr val="accent6">
                     <a:shade val="90000"/>
                     <a:lumMod val="90000"/>
                   </a:schemeClr>
@@ -2083,6 +2190,61 @@
             </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Process!$C$2:$C$5</c:f>
@@ -2133,7 +2295,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2154,15 +2316,13 @@
                   <a:gradFill rotWithShape="1">
                     <a:gsLst>
                       <a:gs pos="0">
-                        <a:schemeClr val="accent2">
-                          <a:shade val="86000"/>
+                        <a:schemeClr val="accent4">
                           <a:tint val="96000"/>
                           <a:lumMod val="104000"/>
                         </a:schemeClr>
                       </a:gs>
                       <a:gs pos="100000">
-                        <a:schemeClr val="accent2">
-                          <a:shade val="86000"/>
+                        <a:schemeClr val="accent4">
                           <a:shade val="90000"/>
                           <a:lumMod val="90000"/>
                         </a:schemeClr>
@@ -2193,6 +2353,61 @@
                   </a:sp3d>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="85000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="95000"/>
+                                <a:alpha val="54000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
                     <c:extLst>
@@ -2254,14 +2469,14 @@
                     <a:gsLst>
                       <a:gs pos="0">
                         <a:schemeClr val="accent2">
-                          <a:tint val="58000"/>
+                          <a:lumMod val="60000"/>
                           <a:tint val="96000"/>
                           <a:lumMod val="104000"/>
                         </a:schemeClr>
                       </a:gs>
                       <a:gs pos="100000">
                         <a:schemeClr val="accent2">
-                          <a:tint val="58000"/>
+                          <a:lumMod val="60000"/>
                           <a:shade val="90000"/>
                           <a:lumMod val="90000"/>
                         </a:schemeClr>
@@ -2292,6 +2507,61 @@
                   </a:sp3d>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="85000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="95000"/>
+                                <a:alpha val="54000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
@@ -2618,7 +2888,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Walmart</c:v>
+            <c:strRef>
+              <c:f>Process!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Walmart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
@@ -2702,7 +2980,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Costco</c:v>
+            <c:strRef>
+              <c:f>Process!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Costco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
@@ -3234,7 +3520,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Walmart</c:v>
+            <c:strRef>
+              <c:f>Process!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Walmart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3359,7 +3653,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Costco</c:v>
+            <c:strRef>
+              <c:f>Process!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Costco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -4055,7 +4357,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Walmart</c:v>
+            <c:strRef>
+              <c:f>Process!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Walmart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -4175,7 +4485,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Costco</c:v>
+            <c:strRef>
+              <c:f>Process!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Costco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -4794,7 +5112,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Walmart</c:v>
+            <c:strRef>
+              <c:f>Process!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Walmart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:noFill/>
@@ -4922,7 +5248,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Costco</c:v>
+            <c:strRef>
+              <c:f>Process!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Costco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:noFill/>
@@ -5588,8 +5922,39 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -9248,7 +9613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="61" zoomScaleNormal="176" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="176" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -9262,564 +9627,564 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="31">
         <v>45138</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="32">
         <v>45046</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="33">
         <v>44957</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="32">
         <v>44865</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="35">
         <v>39782000</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="36">
         <v>37017000</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="36">
         <v>38625000</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="36">
         <v>37200000</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="37">
         <v>255121000</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="38">
         <v>245053000</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="38">
         <v>243457000</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="38">
         <v>247656000</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="37">
         <v>169562000</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="38">
         <v>165588000</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="38">
         <v>159466000</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="38">
         <v>167273000</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="37">
         <v>85559000</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="38">
         <v>79465000</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="38">
         <v>83991000</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="38">
         <v>80383000</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="37">
         <v>14041000</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="38">
         <v>7891000</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="38">
         <v>1673000</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="38">
         <v>6275000</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="37">
         <v>13568000</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="38">
         <v>4633000</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="38">
         <v>13403000</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="38">
         <v>6458000</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="40">
         <v>3270000</v>
       </c>
-      <c r="C9" s="50">
+      <c r="C9" s="41">
         <v>1713000</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="41">
         <v>-2812000</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="41">
         <v>-2104000</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="31">
         <v>44957</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="42">
         <v>44592</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="42">
         <v>44227</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="42">
         <v>43861</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="35">
         <v>147568000</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="36">
         <v>143754000</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="36">
         <v>138836000</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="36">
         <v>129359000</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="37">
         <v>243457000</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="38">
         <v>244860000</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="38">
         <v>252496000</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="38">
         <v>236495000</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="37">
         <v>159466000</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="38">
         <v>152969000</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="38">
         <v>164965000</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="38">
         <v>154943000</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="37">
         <v>76693000</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="38">
         <v>83253000</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="38">
         <v>81298000</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="38">
         <v>74669000</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="53">
+      <c r="B15" s="44">
         <v>11680000</v>
       </c>
-      <c r="C15" s="47">
+      <c r="C15" s="38">
         <v>13673000</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="38">
         <v>13510000</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="38">
         <v>14881000</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="46">
+      <c r="B16" s="37">
         <v>29101000</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="38">
         <v>24181000</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="38">
         <v>36074000</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="38">
         <v>25255000</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B17" s="37">
         <v>-5660000</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="38">
         <v>-4662000</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="38">
         <v>9886000</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="38">
         <v>1828000</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="54">
+      <c r="B19" s="45">
         <v>45169</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="32">
         <v>45077</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="33">
         <v>44985</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="32">
         <v>44957</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="35">
         <v>9720000</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="36">
         <v>6473000</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="36">
         <v>6843000</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="36">
         <v>6843000</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="46">
+      <c r="B21" s="37">
         <v>68994000</v>
       </c>
-      <c r="C21" s="47">
+      <c r="C21" s="38">
         <v>66752000</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="38">
         <v>66848000</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="38">
         <v>66848000</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="46">
+      <c r="B22" s="37">
         <v>43936000</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="38">
         <v>43179000</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="38">
         <v>44049000</v>
       </c>
-      <c r="E22" s="47">
+      <c r="E22" s="38">
         <v>44049000</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="46">
+      <c r="B23" s="37">
         <v>25058000</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="38">
         <v>23568000</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D23" s="38">
         <v>22794000</v>
       </c>
-      <c r="E23" s="47">
+      <c r="E23" s="38">
         <v>22794000</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="46">
+      <c r="B24" s="37">
         <v>6292000</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="38">
         <v>2160000</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D24" s="38">
         <v>1302000</v>
       </c>
-      <c r="E24" s="47">
+      <c r="E24" s="38">
         <v>1466000</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="46">
+      <c r="B25" s="37">
         <v>3725000</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="38">
         <v>1541000</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="38">
         <v>3192000</v>
       </c>
-      <c r="E25" s="47">
+      <c r="E25" s="38">
         <v>2610000</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="49">
+      <c r="B26" s="40">
         <v>1236000</v>
       </c>
-      <c r="C26" s="50">
+      <c r="C26" s="41">
         <v>-476000</v>
       </c>
-      <c r="D26" s="50">
+      <c r="D26" s="41">
         <v>2032000</v>
       </c>
-      <c r="E26" s="50">
+      <c r="E26" s="41">
         <v>690000</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="54">
+      <c r="B27" s="45">
         <v>45169</v>
       </c>
-      <c r="C27" s="51">
+      <c r="C27" s="42">
         <v>44804</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="42">
         <v>44439</v>
       </c>
-      <c r="E27" s="51">
+      <c r="E27" s="42">
         <v>44074</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="44">
+      <c r="B28" s="35">
         <v>29704000</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="36">
         <v>27572000</v>
       </c>
-      <c r="D28" s="45">
+      <c r="D28" s="36">
         <v>25245000</v>
       </c>
-      <c r="E28" s="45">
+      <c r="E28" s="36">
         <v>21822000</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="46">
+      <c r="B29" s="37">
         <v>68994000</v>
       </c>
-      <c r="C29" s="47">
+      <c r="C29" s="38">
         <v>64166000</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="38">
         <v>59268000</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="38">
         <v>55556000</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="46">
+      <c r="B30" s="37">
         <v>43936000</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="38">
         <v>43519000</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="38">
         <v>41190000</v>
       </c>
-      <c r="E30" s="47">
+      <c r="E30" s="38">
         <v>36851000</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="46">
+      <c r="B31" s="37">
         <v>25058000</v>
       </c>
-      <c r="C31" s="47">
+      <c r="C31" s="38">
         <v>20642000</v>
       </c>
-      <c r="D31" s="47">
+      <c r="D31" s="38">
         <v>17564000</v>
       </c>
-      <c r="E31" s="47">
+      <c r="E31" s="38">
         <v>18284000</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="53">
+      <c r="B32" s="44">
         <v>6292000</v>
       </c>
-      <c r="C32" s="47">
+      <c r="C32" s="38">
         <v>5844000</v>
       </c>
-      <c r="D32" s="47">
+      <c r="D32" s="38">
         <v>5007000</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="38">
         <v>4002000</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="46">
+      <c r="B33" s="37">
         <v>11068000</v>
       </c>
-      <c r="C33" s="47">
+      <c r="C33" s="38">
         <v>7392000</v>
       </c>
-      <c r="D33" s="47">
+      <c r="D33" s="38">
         <v>8958000</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="38">
         <v>8861000</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="37">
         <v>3482000</v>
       </c>
-      <c r="C34" s="47">
+      <c r="C34" s="38">
         <v>-806000</v>
       </c>
-      <c r="D34" s="47">
+      <c r="D34" s="38">
         <v>-1065000</v>
       </c>
-      <c r="E34" s="47">
+      <c r="E34" s="38">
         <v>3823000</v>
       </c>
     </row>
@@ -9837,10 +10202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EC2443-40CB-446D-BB83-686BA2887BDC}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="I1" zoomScale="57" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -9848,8 +10213,8 @@
     <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.26953125" bestFit="1" customWidth="1"/>
@@ -9857,798 +10222,866 @@
     <col min="10" max="10" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:15" ht="23.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="109"/>
+      <c r="L1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="32" t="s">
+      <c r="M1" s="109"/>
+      <c r="N1" s="24" t="s">
         <v>22</v>
       </c>
+      <c r="O1" s="112" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="15">
         <f>'Data Collection'!$B$10</f>
         <v>44957</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="16">
         <f>'Data Collection'!$B$11</f>
         <v>147568000</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="16">
         <f>'Data Collection'!$B$12</f>
         <v>243457000</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="16">
         <f>'Data Collection'!$D$13</f>
         <v>164965000</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="16">
         <f>'Data Collection'!$B$13</f>
         <v>159466000</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="16">
         <f>'Data Collection'!$B$15</f>
         <v>11680000</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="16">
         <f>'Data Collection'!$B$16</f>
         <v>29101000</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="16">
         <f>'Data Collection'!$B$17</f>
         <v>-5660000</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="19">
-        <f>'Data Collection'!$B$13</f>
-        <v>159466000</v>
-      </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="20">
+      <c r="K2" s="110"/>
+      <c r="L2" s="16">
+        <f>E2-F2</f>
+        <v>78492000</v>
+      </c>
+      <c r="M2" s="110"/>
+      <c r="N2" s="17">
         <f>Process!H2/Process!E2</f>
         <v>4.7975617870917656E-2</v>
       </c>
+      <c r="O2" s="17">
+        <f>H2/G2</f>
+        <v>7.3244453363099343E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="18">
+    <row r="3" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="15">
         <f>'Data Collection'!$C$10</f>
         <v>44592</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="16">
         <f>'Data Collection'!$C$11</f>
         <v>143754000</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="16">
         <f>'Data Collection'!$C$12</f>
         <v>244860000</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="16">
         <f>'Data Collection'!$C$13</f>
         <v>152969000</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="16">
         <f>'Data Collection'!$C$14</f>
         <v>83253000</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="16">
         <f>'Data Collection'!$C$15</f>
         <v>13673000</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="16">
         <f>'Data Collection'!$C$16</f>
         <v>24181000</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="16">
         <f>'Data Collection'!$C$17</f>
         <v>-4662000</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="19">
-        <f>'Data Collection'!$C$14</f>
-        <v>83253000</v>
-      </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="20">
+      <c r="K3" s="110"/>
+      <c r="L3" s="16">
+        <f>E3-F3</f>
+        <v>91891000</v>
+      </c>
+      <c r="M3" s="110"/>
+      <c r="N3" s="17">
         <f>Process!H3/Process!E3</f>
         <v>5.5840071877807727E-2</v>
       </c>
+      <c r="O3" s="17">
+        <f>H3/G3</f>
+        <v>0.16423432188629838</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="18">
+    <row r="4" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="15">
         <f>'Data Collection'!$D$10</f>
         <v>44227</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <f>'Data Collection'!$D$11</f>
         <v>138836000</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <f>'Data Collection'!$C$12</f>
         <v>244860000</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="16">
         <f>'Data Collection'!$D$13</f>
         <v>164965000</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <f>'Data Collection'!$D$14</f>
         <v>81298000</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="16">
         <f>'Data Collection'!$D$15</f>
         <v>13510000</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="16">
         <f>'Data Collection'!$D$16</f>
         <v>36074000</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="16">
         <f>'Data Collection'!$D$17</f>
         <v>9886000</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="19">
-        <f>'Data Collection'!$D$14</f>
-        <v>81298000</v>
-      </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="20">
+      <c r="K4" s="110"/>
+      <c r="L4" s="16">
+        <f>E4-F4</f>
+        <v>79895000</v>
+      </c>
+      <c r="M4" s="110"/>
+      <c r="N4" s="17">
         <f>Process!H4 / Process!E4</f>
         <v>5.5174385363064606E-2</v>
       </c>
+      <c r="O4" s="17">
+        <f>H4/G4</f>
+        <v>0.16617874978474256</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="18">
+    <row r="5" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="15">
         <f>'Data Collection'!$E$10</f>
         <v>43861</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <f>'Data Collection'!$E$11</f>
         <v>129359000</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="16">
         <f>'Data Collection'!$E$12</f>
         <v>236495000</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <f>'Data Collection'!$E$13</f>
         <v>154943000</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <f>'Data Collection'!$E$14</f>
         <v>74669000</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <f>'Data Collection'!$E$15</f>
         <v>14881000</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="16">
         <f>'Data Collection'!$E$16</f>
         <v>25255000</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="16">
         <f>'Data Collection'!$E$17</f>
         <v>1828000</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="19">
-        <f>'Data Collection'!$E$14</f>
-        <v>74669000</v>
-      </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="20">
+      <c r="K5" s="110"/>
+      <c r="L5" s="16">
+        <f>E5-F5</f>
+        <v>81552000</v>
+      </c>
+      <c r="M5" s="110"/>
+      <c r="N5" s="17">
         <f>Process!H5 / Process!E5</f>
         <v>6.2923106196748346E-2</v>
       </c>
+      <c r="O5" s="17">
+        <f>H5/G5</f>
+        <v>0.19929287924038089</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35" t="s">
+    <row r="6" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="101">
         <f>'Data Collection'!$B$2</f>
         <v>45138</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="102">
         <f>'Data Collection'!$B$3</f>
         <v>39782000</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="102">
         <f>'Data Collection'!$B$4</f>
         <v>255121000</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="102">
         <f>'Data Collection'!$B$5</f>
         <v>169562000</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="102">
         <f>'Data Collection'!$B$6</f>
         <v>85559000</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="102">
         <f>'Data Collection'!$B$7</f>
         <v>14041000</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="102">
         <f>'Data Collection'!$B$8</f>
         <v>13568000</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="102">
         <f>'Data Collection'!$B$9</f>
         <v>3270000</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="19">
-        <f>'Data Collection'!$B$6</f>
+      <c r="K6" s="110"/>
+      <c r="L6" s="102">
+        <f>E6-F6</f>
         <v>85559000</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="20">
+      <c r="M6" s="110"/>
+      <c r="N6" s="105">
         <f>Process!H6 / Process!E6</f>
         <v>5.5036629677682351E-2</v>
       </c>
+      <c r="O6" s="105">
+        <f>H6/G6</f>
+        <v>0.16410897743077876</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="18">
+    <row r="7" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="101">
         <f>'Data Collection'!$C$2</f>
         <v>45046</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="102">
         <f>'Data Collection'!$C$3</f>
         <v>37017000</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="102">
         <f>'Data Collection'!$C$4</f>
         <v>245053000</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="102">
         <f>'Data Collection'!$C$5</f>
         <v>165588000</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="102">
         <f>'Data Collection'!$C$6</f>
         <v>79465000</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="102">
         <f>'Data Collection'!$C$7</f>
         <v>7891000</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="102">
         <f>'Data Collection'!$C$8</f>
         <v>4633000</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="102">
         <f>'Data Collection'!$C$9</f>
         <v>1713000</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="19">
-        <f>'Data Collection'!$C$6</f>
+      <c r="K7" s="110"/>
+      <c r="L7" s="102">
+        <f>E7-F7</f>
         <v>79465000</v>
       </c>
-      <c r="M7" s="17"/>
-      <c r="N7" s="20">
+      <c r="M7" s="110"/>
+      <c r="N7" s="105">
         <f>Process!H7 / Process!E7</f>
         <v>3.2201197292014379E-2</v>
       </c>
+      <c r="O7" s="105">
+        <f>H7/G7</f>
+        <v>9.930157931164664E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="18">
+    <row r="8" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="101">
         <f>'Data Collection'!$D$2</f>
         <v>44957</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="102">
         <f>'Data Collection'!$D$3</f>
         <v>38625000</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="102">
         <f>'Data Collection'!$D$4</f>
         <v>243457000</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="102">
         <f>'Data Collection'!$D$5</f>
         <v>159466000</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="102">
         <f>'Data Collection'!$D$6</f>
         <v>83991000</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="102">
         <f>'Data Collection'!$D$7</f>
         <v>1673000</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="102">
         <f>'Data Collection'!$D$8</f>
         <v>13403000</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="102">
         <f>'Data Collection'!$D$9</f>
         <v>-2812000</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="19">
-        <f>'Data Collection'!$D$6</f>
+      <c r="K8" s="110"/>
+      <c r="L8" s="102">
+        <f>E8-F8</f>
         <v>83991000</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="N8" s="20">
+      <c r="M8" s="110"/>
+      <c r="N8" s="105">
         <f>H8 / E8</f>
         <v>6.8718500597641473E-3</v>
       </c>
+      <c r="O8" s="105">
+        <f>H8/G8</f>
+        <v>1.9918800823897798E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="21">
+    <row r="9" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="103">
         <f>'Data Collection'!$E$2</f>
         <v>44865</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="104">
         <f>'Data Collection'!$E$3</f>
         <v>37200000</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="104">
         <f>'Data Collection'!$E$4</f>
         <v>247656000</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="104">
         <f>'Data Collection'!$E$5</f>
         <v>167273000</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="104">
         <f>'Data Collection'!$E$6</f>
         <v>80383000</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="104">
         <f>'Data Collection'!$E$7</f>
         <v>6275000</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="104">
         <f>'Data Collection'!$E$8</f>
         <v>6458000</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="104">
         <f>'Data Collection'!$E$9</f>
         <v>-2104000</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="22">
-        <f>'Data Collection'!$E$6</f>
+      <c r="K9" s="110"/>
+      <c r="L9" s="104">
+        <f>E9-F9</f>
         <v>80383000</v>
       </c>
-      <c r="M9" s="17"/>
-      <c r="N9" s="23">
+      <c r="M9" s="110"/>
+      <c r="N9" s="106">
         <f>Process!H9 / Process!E9</f>
         <v>2.5337565009529345E-2</v>
       </c>
+      <c r="O9" s="107">
+        <f>H9/G9</f>
+        <v>7.8063769702549052E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="34" t="s">
+    <row r="10" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="18">
         <f>'Data Collection'!$B$27</f>
         <v>45169</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="19">
         <f>'Data Collection'!$B$28</f>
         <v>29704000</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="19">
         <f>'Data Collection'!$B$29</f>
         <v>68994000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="19">
         <f>'Data Collection'!$B$30</f>
         <v>43936000</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="19">
         <f>'Data Collection'!$B$31</f>
         <v>25058000</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="19">
         <f>'Data Collection'!$B$32</f>
         <v>6292000</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="19">
         <f>'Data Collection'!$B$33</f>
         <v>11068000</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="19">
         <f>'Data Collection'!$B$34</f>
         <v>3482000</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="25">
-        <f>'Data Collection'!$B$31</f>
+      <c r="K10" s="110"/>
+      <c r="L10" s="19">
+        <f>E10-F10</f>
         <v>25058000</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="26">
+      <c r="M10" s="110"/>
+      <c r="N10" s="20">
         <f>Process!H10/Process!E10</f>
         <v>9.1196335913267826E-2</v>
       </c>
+      <c r="O10" s="111">
+        <f>H10/G10</f>
+        <v>0.25109745390693589</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="18">
+    <row r="11" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="15">
         <f>'Data Collection'!$C$27</f>
         <v>44804</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="16">
         <f>'Data Collection'!$C$28</f>
         <v>27572000</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="16">
         <f>'Data Collection'!$C$29</f>
         <v>64166000</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="16">
         <f>'Data Collection'!$C$30</f>
         <v>43519000</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <f>'Data Collection'!$C$31</f>
         <v>20642000</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="16">
         <f>'Data Collection'!$C$32</f>
         <v>5844000</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="16">
         <f>'Data Collection'!$C$33</f>
         <v>7392000</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="16">
         <f>'Data Collection'!$C$34</f>
         <v>-806000</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="19">
-        <f>'Data Collection'!$C$31</f>
-        <v>20642000</v>
-      </c>
-      <c r="M11" s="17"/>
-      <c r="N11" s="20">
+      <c r="K11" s="110"/>
+      <c r="L11" s="16">
+        <f>E11-F11</f>
+        <v>20647000</v>
+      </c>
+      <c r="M11" s="110"/>
+      <c r="N11" s="17">
         <f>Process!H11/Process!E11</f>
         <v>9.1076270922295297E-2</v>
       </c>
+      <c r="O11" s="17">
+        <f>H11/G11</f>
+        <v>0.28311210154054839</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="18">
+    <row r="12" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="15">
         <f>'Data Collection'!$D$27</f>
         <v>44439</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="16">
         <f>'Data Collection'!$D$28</f>
         <v>25245000</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="16">
         <f>'Data Collection'!$D$29</f>
         <v>59268000</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="16">
         <f>'Data Collection'!$D$30</f>
         <v>41190000</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <f>'Data Collection'!$D$31</f>
         <v>17564000</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="16">
         <f>'Data Collection'!$D$32</f>
         <v>5007000</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="16">
         <f>'Data Collection'!$D$33</f>
         <v>8958000</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="16">
         <f>'Data Collection'!$D$34</f>
         <v>-1065000</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="19">
-        <f>'Data Collection'!$D$31</f>
-        <v>17564000</v>
-      </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="20">
+      <c r="K12" s="110"/>
+      <c r="L12" s="16">
+        <f>E12-F12</f>
+        <v>18078000</v>
+      </c>
+      <c r="M12" s="110"/>
+      <c r="N12" s="17">
         <f>Process!H12 / Process!E12</f>
         <v>8.4480664102044953E-2</v>
       </c>
+      <c r="O12" s="17">
+        <f>H12/G12</f>
+        <v>0.28507173764518334</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="18">
+    <row r="13" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="15">
         <f>'Data Collection'!$E$27</f>
         <v>44074</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <f>'Data Collection'!$E$28</f>
         <v>21822000</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="16">
         <f>'Data Collection'!$E$29</f>
         <v>55556000</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="16">
         <f>'Data Collection'!$E$30</f>
         <v>36851000</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <f>'Data Collection'!$E$31</f>
         <v>18284000</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="16">
         <f>'Data Collection'!$E$32</f>
         <v>4002000</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="16">
         <f>'Data Collection'!$E$33</f>
         <v>8861000</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="16">
         <f>'Data Collection'!$E$34</f>
         <v>3823000</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="19">
-        <f>'Data Collection'!$E$31</f>
-        <v>18284000</v>
-      </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="20">
+      <c r="K13" s="110"/>
+      <c r="L13" s="16">
+        <f>E13-F13</f>
+        <v>18705000</v>
+      </c>
+      <c r="M13" s="110"/>
+      <c r="N13" s="17">
         <f>Process!H13 / Process!E13</f>
         <v>7.2035423716610272E-2</v>
       </c>
+      <c r="O13" s="17">
+        <f>H13/G13</f>
+        <v>0.21887989499015534</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="34"/>
-      <c r="B14" s="35" t="s">
+    <row r="14" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="101">
         <f>'Data Collection'!$B$19</f>
         <v>45169</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="102">
         <f>'Data Collection'!$B$20</f>
         <v>9720000</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="102">
         <f>'Data Collection'!$B$21</f>
         <v>68994000</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="102">
         <f>'Data Collection'!$B$22</f>
         <v>43936000</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="102">
         <f>'Data Collection'!$B$23</f>
         <v>25058000</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="102">
         <f>'Data Collection'!$B$24</f>
         <v>6292000</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="102">
         <f>'Data Collection'!$B$25</f>
         <v>3725000</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="102">
         <f>'Data Collection'!$B$26</f>
         <v>1236000</v>
       </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="19">
-        <f>'Data Collection'!$B$23</f>
+      <c r="K14" s="110"/>
+      <c r="L14" s="102">
+        <f>E14-F14</f>
         <v>25058000</v>
       </c>
-      <c r="M14" s="17"/>
-      <c r="N14" s="20">
+      <c r="M14" s="110"/>
+      <c r="N14" s="105">
         <f>Process!H14 / Process!E14</f>
         <v>9.1196335913267826E-2</v>
       </c>
+      <c r="O14" s="105">
+        <f>H14/G14</f>
+        <v>0.25109745390693589</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="18">
+    <row r="15" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="101">
         <f>'Data Collection'!$C$19</f>
         <v>45077</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="102">
         <f>'Data Collection'!$C$20</f>
         <v>6473000</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="102">
         <f>'Data Collection'!$C$21</f>
         <v>66752000</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="102">
         <f>'Data Collection'!$C$22</f>
         <v>43179000</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="102">
         <f>'Data Collection'!$C$23</f>
         <v>23568000</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="102">
         <f>'Data Collection'!$C$24</f>
         <v>2160000</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="102">
         <f>'Data Collection'!$C$25</f>
         <v>1541000</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="102">
         <f>'Data Collection'!$C$26</f>
         <v>-476000</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="19">
-        <f>'Data Collection'!$C$23</f>
-        <v>23568000</v>
-      </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="20">
+      <c r="K15" s="110"/>
+      <c r="L15" s="102">
+        <f>E15-F15</f>
+        <v>23573000</v>
+      </c>
+      <c r="M15" s="110"/>
+      <c r="N15" s="105">
         <f>Process!H15 / Process!E15</f>
         <v>3.235858101629914E-2</v>
       </c>
+      <c r="O15" s="105">
+        <f>H15/G15</f>
+        <v>9.1649694501018328E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="18">
+    <row r="16" spans="1:15" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="101">
         <f>'Data Collection'!$D$19</f>
         <v>44985</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="102">
         <f>'Data Collection'!$D$20</f>
         <v>6843000</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="102">
         <f>'Data Collection'!$D$21</f>
         <v>66848000</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="102">
         <f>'Data Collection'!$D$22</f>
         <v>44049000</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="102">
         <f>'Data Collection'!$D$23</f>
         <v>22794000</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="102">
         <f>'Data Collection'!$D$24</f>
         <v>1302000</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="102">
         <f>'Data Collection'!$D$25</f>
         <v>3192000</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="102">
         <f>'Data Collection'!$D$26</f>
         <v>2032000</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="19">
-        <f>'Data Collection'!$D$23</f>
-        <v>22794000</v>
-      </c>
-      <c r="M16" s="17"/>
-      <c r="N16" s="27">
+      <c r="K16" s="110"/>
+      <c r="L16" s="102">
+        <f>E16-F16</f>
+        <v>22799000</v>
+      </c>
+      <c r="M16" s="110"/>
+      <c r="N16" s="107">
         <f>H16 / E16</f>
         <v>1.9477022498803256E-2</v>
       </c>
+      <c r="O16" s="105">
+        <f>H16/G16</f>
+        <v>5.7120294814424849E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" ht="27.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="18">
+    <row r="17" spans="1:15" ht="27.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="101">
         <f>'Data Collection'!$E$19</f>
         <v>44957</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="102">
         <f>'Data Collection'!$E$20</f>
         <v>6843000</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="102">
         <f>'Data Collection'!$E$21</f>
         <v>66848000</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="102">
         <f>'Data Collection'!$E$22</f>
         <v>44049000</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="102">
         <f>'Data Collection'!$E$23</f>
         <v>22794000</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="102">
         <f>'Data Collection'!$E$24</f>
         <v>1466000</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="102">
         <f>'Data Collection'!$E$25</f>
         <v>2610000</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="102">
         <f>'Data Collection'!$E$26</f>
         <v>690000</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="19">
-        <f>'Data Collection'!$E$23</f>
-        <v>22794000</v>
-      </c>
-      <c r="M17" s="17"/>
-      <c r="N17" s="28">
+      <c r="K17" s="110"/>
+      <c r="L17" s="102">
+        <f>E17-F17</f>
+        <v>22799000</v>
+      </c>
+      <c r="M17" s="110"/>
+      <c r="N17" s="108">
         <f>Process!H17 / Process!E17</f>
         <v>2.1930349449497368E-2</v>
       </c>
+      <c r="O17" s="105">
+        <f>H17/G17</f>
+        <v>6.4315170658945334E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
     </row>
   </sheetData>
@@ -10670,8 +11103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1D3D86-40A7-4240-9003-D7BBC33CF772}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="A26" zoomScale="65" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10688,556 +11121,556 @@
     <row r="2" spans="1:8" ht="14" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="105"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="96"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="107"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="98"/>
     </row>
     <row r="4" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="109"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="15" t="str">
+      <c r="C5" s="13" t="str">
         <f>Process!A2 &amp;CHAR(10)&amp;COUNTIF(C11:C42, "Pass*") &amp; " out of " &amp; COUNTIF(C11:C42, "Pass*")+COUNTIF(C11:C42, "Fail*")</f>
         <v>Walmart
 7 out of 8</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="str">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="str">
         <f>Process!A10 &amp;CHAR(10)&amp;COUNTIF(F12:F42, "Pass*") &amp; " out of " &amp; COUNTIF(F12:F42, "Pass*")+COUNTIF(F12:F42, "Fail*")</f>
         <v>Costco
 7 out of 8</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
     </row>
     <row r="12" spans="1:8" ht="23.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="55" t="str">
+      <c r="B13" s="58"/>
+      <c r="C13" s="46" t="str">
         <f>IF(Process!H9 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D13" s="56" t="str">
+      <c r="D13" s="47" t="str">
         <f>DOLLAR(Process!H9,0)</f>
         <v>$6,275,000</v>
       </c>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55" t="str">
+      <c r="E13" s="46"/>
+      <c r="F13" s="46" t="str">
         <f>IF(Process!H17 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G13" s="56" t="str">
+      <c r="G13" s="47" t="str">
         <f>DOLLAR(Process!H17,0)</f>
         <v>$1,466,000</v>
       </c>
-      <c r="H13" s="55"/>
+      <c r="H13" s="46"/>
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="67"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="55" t="str">
+      <c r="B15" s="58"/>
+      <c r="C15" s="46" t="str">
         <f>IF(Process!I9 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D15" s="56" t="str">
+      <c r="D15" s="47" t="str">
         <f>DOLLAR(Process!I9,0)</f>
         <v>$6,458,000</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55" t="str">
+      <c r="E15" s="46"/>
+      <c r="F15" s="46" t="str">
         <f>IF(Process!I17 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G15" s="56" t="str">
+      <c r="G15" s="47" t="str">
         <f>DOLLAR(Process!I17,0)</f>
         <v>$2,610,000</v>
       </c>
-      <c r="H15" s="55"/>
+      <c r="H15" s="46"/>
     </row>
     <row r="16" spans="1:8" ht="22" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="67"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="55" t="str">
+      <c r="B17" s="58"/>
+      <c r="C17" s="46" t="str">
         <f>IF(Process!N9 &gt; 1%, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="48">
         <f>Process!N9</f>
         <v>2.5337565009529345E-2</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="55" t="str">
+      <c r="E17" s="48"/>
+      <c r="F17" s="46" t="str">
         <f>IF(Process!N17 &gt; 1%, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G17" s="57">
+      <c r="G17" s="48">
         <f>Process!N17</f>
         <v>2.1930349449497368E-2</v>
       </c>
-      <c r="H17" s="55"/>
+      <c r="H17" s="46"/>
     </row>
     <row r="18" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="67"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
     </row>
     <row r="19" spans="1:8" ht="18.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="58" t="str">
+      <c r="B19" s="61"/>
+      <c r="C19" s="49" t="str">
         <f>IF(Process!I9 &gt; Process!H9, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D19" s="59" t="str">
+      <c r="D19" s="50" t="str">
         <f>"Cash Flow= " &amp; DOLLAR(Process!I9,0) &amp;CHAR(10)&amp; " Net Income= " &amp; DOLLAR(Process!H9,0)</f>
         <v>Cash Flow= $6,458,000
  Net Income= $6,275,000</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="58" t="str">
+      <c r="E19" s="51"/>
+      <c r="F19" s="49" t="str">
         <f>IF(Process!I17 &gt; Process!H17, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G19" s="59" t="str">
+      <c r="G19" s="50" t="str">
         <f>"Cash Flow= " &amp; DOLLAR(Process!I17,0) &amp;CHAR(10)&amp; " Net Income= " &amp; DOLLAR(Process!H17,0)</f>
         <v>Cash Flow= $2,610,000
  Net Income= $1,466,000</v>
       </c>
-      <c r="H19" s="60"/>
+      <c r="H19" s="51"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="63"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="54"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="66"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="9" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="12.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="94"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="97"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="88"/>
     </row>
     <row r="26" spans="1:8" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="100"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="67" t="s">
+      <c r="A27" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="58" t="str">
+      <c r="B27" s="58"/>
+      <c r="C27" s="49" t="str">
         <f>IF(Process!E9 &gt; Process!F9, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D27" s="59" t="str">
+      <c r="D27" s="50" t="str">
         <f>"Assets = " &amp; DOLLAR(Process!E9,0) &amp; CHAR(10)&amp; " Liabilities = "&amp;DOLLAR(Process!F9,0)</f>
         <v>Assets = $247,656,000
  Liabilities = $167,273,000</v>
       </c>
-      <c r="E27" s="60"/>
-      <c r="F27" s="58" t="str">
+      <c r="E27" s="51"/>
+      <c r="F27" s="49" t="str">
         <f>IF(Process!E17 &gt; Process!F17, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G27" s="59" t="str">
+      <c r="G27" s="50" t="str">
         <f>"Assets = " &amp; DOLLAR(Process!E17,0) &amp; CHAR(10)&amp; " Liabilities = "&amp;DOLLAR(Process!F17,0)</f>
         <v>Assets = $66,848,000
  Liabilities = $44,049,000</v>
       </c>
-      <c r="H27" s="60"/>
+      <c r="H27" s="51"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="67"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="63"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="54"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="67"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="66"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="57"/>
     </row>
     <row r="30" spans="1:8" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="58" t="str">
+      <c r="B30" s="58"/>
+      <c r="C30" s="49" t="str">
         <f>IF(Process!L9 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D30" s="82" t="str">
+      <c r="D30" s="73" t="str">
         <f>DOLLAR(Process!L9,0)</f>
         <v>$80,383,000</v>
       </c>
-      <c r="E30" s="83"/>
-      <c r="F30" s="58" t="str">
+      <c r="E30" s="74"/>
+      <c r="F30" s="49" t="str">
         <f>IF(Process!L17 &gt; 0, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G30" s="82" t="str">
+      <c r="G30" s="73" t="str">
         <f>DOLLAR(Process!L17,0)</f>
-        <v>$22,794,000</v>
-      </c>
-      <c r="H30" s="83"/>
+        <v>$22,799,000</v>
+      </c>
+      <c r="H30" s="74"/>
     </row>
     <row r="31" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="67"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="84"/>
-      <c r="H31" s="85"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="76"/>
     </row>
     <row r="32" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="75"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="8" t="s">
+      <c r="A32" s="66"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="75"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="75"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="91" t="s">
+      <c r="A34" s="66"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
     </row>
     <row r="35" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="91"/>
-      <c r="H35" s="91"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
     </row>
     <row r="36" spans="1:8" ht="35.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="75"/>
-      <c r="B36" s="75"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="91"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
     </row>
     <row r="37" spans="1:8" ht="24.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="76" t="s">
+      <c r="A37" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="5" t="str">
+      <c r="B37" s="68"/>
+      <c r="C37" s="113" t="str">
         <f>IF(Process!D9 &gt; 0, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="D37" s="7" t="str">
+      <c r="D37" s="114" t="str">
         <f>DOLLAR(Process!D9,0)</f>
         <v>$37,200,000</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="5" t="str">
+      <c r="E37" s="114"/>
+      <c r="F37" s="113" t="str">
         <f>IF(Process!D17 &gt; 0, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="G37" s="7" t="str">
+      <c r="G37" s="114" t="str">
         <f>DOLLAR(Process!D17,0)</f>
         <v>$6,843,000</v>
       </c>
-      <c r="H37" s="7"/>
+      <c r="H37" s="114"/>
     </row>
     <row r="38" spans="1:8" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="75"/>
-      <c r="B38" s="75"/>
-      <c r="C38" s="9" t="s">
+      <c r="A38" s="66"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="11"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="75"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="14"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="54.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="75"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="87" t="s">
+      <c r="A40" s="66"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="88"/>
-      <c r="E40" s="88"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="88"/>
-      <c r="H40" s="88"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="78" t="s">
+      <c r="A41" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="79"/>
-      <c r="C41" s="89" t="str">
+      <c r="B41" s="70"/>
+      <c r="C41" s="80" t="str">
         <f>IF(Process!I9 &gt; Process!F9, "Pass", "Fail")</f>
         <v>Fail</v>
       </c>
-      <c r="D41" s="90" t="str">
+      <c r="D41" s="81" t="str">
         <f>"Cash Flow = " &amp; DOLLAR(Process!I9, 0) &amp; CHAR(10)&amp; " Liabilities = " &amp; DOLLAR(Process!F9,0)</f>
         <v>Cash Flow = $6,458,000
  Liabilities = $167,273,000</v>
       </c>
-      <c r="E41" s="90"/>
-      <c r="F41" s="89" t="str">
+      <c r="E41" s="81"/>
+      <c r="F41" s="80" t="str">
         <f>IF(Process!I17 &gt; Process!F17, "Pass", "Fail")</f>
         <v>Fail</v>
       </c>
-      <c r="G41" s="90" t="str">
+      <c r="G41" s="81" t="str">
         <f>"Cash Flow = " &amp; DOLLAR(Process!I17, 0) &amp; CHAR(10)&amp; " Liabilities = " &amp; DOLLAR(Process!F17,0)</f>
         <v>Cash Flow = $2,610,000
  Liabilities = $44,049,000</v>
       </c>
-      <c r="H41" s="90"/>
+      <c r="H41" s="81"/>
     </row>
     <row r="42" spans="1:8" ht="30.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="80"/>
-      <c r="B42" s="81"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="90"/>
-      <c r="E42" s="90"/>
-      <c r="F42" s="89"/>
-      <c r="G42" s="90"/>
-      <c r="H42" s="90"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="81"/>
     </row>
     <row r="43" spans="1:8" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -11300,8 +11733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2C5099-E488-45DC-8972-3201FC9593C4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="58" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView zoomScale="42" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>